<commit_message>
took note of unavailable LM7810CT, switched to LM7810ACT
</commit_message>
<xml_diff>
--- a/Circuit_layout/TSI_BOM.xlsx
+++ b/Circuit_layout/TSI_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="463">
   <si>
     <t>Reference</t>
   </si>
@@ -1405,6 +1405,9 @@
   </si>
   <si>
     <t>IC TRANSCEIVER CAN HI-SPD 8-SOIC</t>
+  </si>
+  <si>
+    <t>Changed to LM7810ACT</t>
   </si>
 </sst>
 </file>
@@ -2239,10 +2242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G165"/>
+  <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3726,7 +3729,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>13</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>113</v>
       </c>
@@ -3772,7 +3775,7 @@
         <v>7.13</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -3795,7 +3798,7 @@
         <v>7.66</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>328</v>
       </c>
@@ -3817,8 +3820,11 @@
       <c r="G68" s="2">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>167</v>
       </c>
@@ -3841,7 +3847,7 @@
         <v>7.79</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>416</v>
       </c>
@@ -3864,7 +3870,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>372</v>
       </c>
@@ -3887,7 +3893,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>358</v>
       </c>
@@ -3910,7 +3916,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>28</v>
       </c>
@@ -3933,7 +3939,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>290</v>
       </c>
@@ -3956,7 +3962,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>259</v>
       </c>
@@ -3979,7 +3985,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>86</v>
       </c>
@@ -4002,7 +4008,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>421</v>
       </c>
@@ -4025,7 +4031,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>57</v>
       </c>
@@ -4048,7 +4054,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>63</v>
       </c>
@@ -4071,7 +4077,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>90</v>
       </c>

</xml_diff>